<commit_message>
sei la o que fiz
</commit_message>
<xml_diff>
--- a/dados/pesquisasGoogle.xlsx
+++ b/dados/pesquisasGoogle.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA50453-B52B-4C9C-A4F6-687E057A4C56}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D954065-5600-4837-A2D1-285B6EF9F149}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>ID</t>
   </si>
@@ -38,6 +38,12 @@
   </si>
   <si>
     <t>Fatec Carapicuiba</t>
+  </si>
+  <si>
+    <t>G_00003</t>
+  </si>
+  <si>
+    <t>RSI</t>
   </si>
 </sst>
 </file>
@@ -425,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,6 +468,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>